<commit_message>
correct units type (thanks MacKenzie!)
</commit_message>
<xml_diff>
--- a/absolute_quant_example.xlsx
+++ b/absolute_quant_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abirmingham/Desktop/absolute_quant/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abirmingham/Work/Repositories/pysyndna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D095F34-6AD4-1B41-8FBC-15982D077CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687F4B58-EE97-5E40-B5B9-6B0F51C3F6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="2340" windowWidth="31480" windowHeight="18180" activeTab="1" xr2:uid="{E184B90C-6432-8947-B7A0-BE1974B73180}"/>
+    <workbookView xWindow="6520" yWindow="1140" windowWidth="31480" windowHeight="18180" xr2:uid="{E184B90C-6432-8947-B7A0-BE1974B73180}"/>
   </bookViews>
   <sheets>
     <sheet name="full_calcs" sheetId="1" r:id="rId1"/>
@@ -1886,11 +1886,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.00000000E+00"/>
-    <numFmt numFmtId="170" formatCode="0.000E+00"/>
-    <numFmt numFmtId="173" formatCode="0.0000000000E+00"/>
-    <numFmt numFmtId="174" formatCode="0.000000000000000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000E+00"/>
+    <numFmt numFmtId="168" formatCode="0.000000000000000E+00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -2095,21 +2095,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -2117,29 +2115,26 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2147,8 +2142,7 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="174" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2166,10 +2160,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2471,9 +2461,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF78FB9F-0C2A-0F43-B368-C0466A3B1D76}">
   <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3272,7 +3262,7 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="G22">
         <f>G21*1000</f>
@@ -3364,10 +3354,10 @@
       <c r="H24">
         <v>100</v>
       </c>
-      <c r="I24" s="17">
+      <c r="I24" s="15">
         <v>70</v>
       </c>
-      <c r="J24" s="17">
+      <c r="J24" s="15">
         <v>70</v>
       </c>
       <c r="K24" t="b">
@@ -3439,13 +3429,13 @@
       <c r="G26">
         <v>2</v>
       </c>
-      <c r="H26" s="40">
+      <c r="H26" s="35">
         <v>1.4</v>
       </c>
-      <c r="I26" s="41">
+      <c r="I26" s="36">
         <v>6</v>
       </c>
-      <c r="J26" s="40">
+      <c r="J26" s="35">
         <v>1.4</v>
       </c>
       <c r="K26" t="b">
@@ -3474,19 +3464,19 @@
       <c r="F27" t="s">
         <v>81</v>
       </c>
-      <c r="G27" s="34">
+      <c r="G27" s="30">
         <f>(G26* G24/G21) * (1/(10^9))</f>
         <v>7.186743134196688E-6</v>
       </c>
-      <c r="H27" s="34">
+      <c r="H27" s="30">
         <f t="shared" ref="H27:J27" si="0">(H26* H24/H21) * (1/(10^9))</f>
         <v>4.7470988923471535E-6</v>
       </c>
-      <c r="I27" s="34">
+      <c r="I27" s="30">
         <f t="shared" si="0"/>
         <v>1.5092160581813043E-5</v>
       </c>
-      <c r="J27" s="34">
+      <c r="J27" s="30">
         <f t="shared" si="0"/>
         <v>3.3229692246430076E-6</v>
       </c>
@@ -3743,16 +3733,16 @@
       <c r="F35" t="s">
         <v>89</v>
       </c>
-      <c r="G35" s="30">
+      <c r="G35" s="27">
         <v>6.0220000000000003E+23</v>
       </c>
-      <c r="H35" s="30">
+      <c r="H35" s="27">
         <v>6.0220000000000003E+23</v>
       </c>
-      <c r="I35" s="30">
+      <c r="I35" s="27">
         <v>6.0220000000000003E+23</v>
       </c>
-      <c r="J35" s="30">
+      <c r="J35" s="27">
         <v>6.0220000000000003E+23</v>
       </c>
       <c r="M35" t="s">
@@ -3830,28 +3820,28 @@
       <c r="B38" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" s="10" t="s">
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
         <v>85</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="E38" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" t="s">
         <v>84</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G38">
         <v>1904788.3330000001</v>
       </c>
-      <c r="H38" s="10">
+      <c r="H38">
         <v>4373730</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I38">
         <v>1904788.3330000001</v>
       </c>
-      <c r="J38" s="10">
+      <c r="J38">
         <v>4373730</v>
       </c>
       <c r="K38" t="b">
@@ -3865,31 +3855,31 @@
       <c r="B39" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" s="10" t="s">
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" t="s">
         <v>13</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" t="s">
         <v>87</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G39" s="5">
         <f>(G37*G$35)/(G38*G$36*10^9)</f>
         <v>263469.80165907741</v>
       </c>
-      <c r="H39" s="12">
+      <c r="H39" s="5">
         <f t="shared" ref="H39:J39" si="2">(H37*H35)/(H38*H36*10^9)</f>
         <v>35419.590158970583</v>
       </c>
-      <c r="I39" s="13">
+      <c r="I39" s="11">
         <f t="shared" si="2"/>
         <v>263469.80165907741</v>
       </c>
-      <c r="J39" s="12">
+      <c r="J39" s="5">
         <f t="shared" si="2"/>
         <v>35419.590158970583</v>
       </c>
@@ -3907,31 +3897,31 @@
       <c r="B40" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D40" s="10" t="s">
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
         <v>95</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" t="s">
         <v>13</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" t="s">
         <v>96</v>
       </c>
-      <c r="G40" s="10">
+      <c r="G40">
         <f>G39/G$30</f>
         <v>52693.960331815484</v>
       </c>
-      <c r="H40" s="10">
+      <c r="H40">
         <f t="shared" ref="H40:J40" si="3">H39/H30</f>
         <v>7441.0903695316356</v>
       </c>
-      <c r="I40" s="11">
+      <c r="I40" s="10">
         <f t="shared" si="3"/>
         <v>52693.960331815484</v>
       </c>
-      <c r="J40" s="10">
+      <c r="J40">
         <f t="shared" si="3"/>
         <v>7441.0903695316356</v>
       </c>
@@ -3946,31 +3936,31 @@
       <c r="B41" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" s="10" t="s">
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" t="s">
         <v>13</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" t="s">
         <v>99</v>
       </c>
-      <c r="G41" s="31">
+      <c r="G41" s="28">
         <f>G40*10^9</f>
         <v>52693960331815.484</v>
       </c>
-      <c r="H41" s="31">
+      <c r="H41" s="28">
         <f t="shared" ref="H41:J41" si="4">H40*10^9</f>
         <v>7441090369531.6357</v>
       </c>
-      <c r="I41" s="33">
+      <c r="I41" s="29">
         <f t="shared" si="4"/>
         <v>52693960331815.484</v>
       </c>
-      <c r="J41" s="31">
+      <c r="J41" s="28">
         <f t="shared" si="4"/>
         <v>7441090369531.6357</v>
       </c>
@@ -3982,34 +3972,34 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" s="15" t="s">
+      <c r="C42" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="G42" s="42">
+      <c r="G42" s="37">
         <f>G41*G$27</f>
         <v>378697957.62830758</v>
       </c>
-      <c r="H42" s="42">
+      <c r="H42" s="37">
         <f t="shared" ref="H42:J42" si="5">H41*H27</f>
         <v>35323591.851058699</v>
       </c>
-      <c r="I42" s="16">
+      <c r="I42" s="14">
         <f t="shared" si="5"/>
         <v>795265711.01944578</v>
       </c>
-      <c r="J42" s="42">
+      <c r="J42" s="37">
         <f t="shared" si="5"/>
         <v>24726514.295741092</v>
       </c>
@@ -4160,19 +4150,19 @@
       <c r="F47" t="s">
         <v>99</v>
       </c>
-      <c r="G47" s="32">
+      <c r="G47" s="28">
         <f>G46*10^9</f>
         <v>27710174830767.367</v>
       </c>
-      <c r="H47" s="32">
+      <c r="H47" s="28">
         <f>H46*10^9</f>
         <v>8987467049815.8281</v>
       </c>
-      <c r="I47" s="32">
+      <c r="I47" s="28">
         <f>I46*10^9</f>
         <v>27710174830767.367</v>
       </c>
-      <c r="J47" s="32">
+      <c r="J47" s="28">
         <f>J46*10^9</f>
         <v>8987467049815.8281</v>
       </c>
@@ -4243,28 +4233,28 @@
       <c r="B50" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C50" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D50" s="10" t="s">
+      <c r="C50" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
         <v>85</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E50" t="s">
         <v>8</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" t="s">
         <v>84</v>
       </c>
-      <c r="G50" s="11">
+      <c r="G50" s="10">
         <v>89264</v>
       </c>
-      <c r="H50" s="11">
+      <c r="H50" s="10">
         <v>89264</v>
       </c>
-      <c r="I50" s="11">
+      <c r="I50" s="10">
         <v>89264</v>
       </c>
-      <c r="J50" s="11">
+      <c r="J50" s="10">
         <v>89264</v>
       </c>
     </row>
@@ -4272,31 +4262,31 @@
       <c r="B51" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" s="10" t="s">
+      <c r="C51" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E51" t="s">
         <v>13</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="F51" t="s">
         <v>87</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="11">
         <f>(G49*G$35)/(G50*G$36*10^9)</f>
         <v>56114.064464876697</v>
       </c>
-      <c r="H51" s="13">
+      <c r="H51" s="11">
         <f>(H49*H$35)/(H50*H$36*10^9)</f>
         <v>17201.133147888297</v>
       </c>
-      <c r="I51" s="13">
+      <c r="I51" s="11">
         <f>(I49*I$35)/(I50*I$36*10^9)</f>
         <v>56114.064464876697</v>
       </c>
-      <c r="J51" s="13">
+      <c r="J51" s="11">
         <f>(J49*J$35)/(J50*J$36*10^9)</f>
         <v>17201.133147888297</v>
       </c>
@@ -4305,31 +4295,31 @@
       <c r="B52" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C52" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D52" s="10" t="s">
+      <c r="C52" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" t="s">
         <v>96</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G52" s="10">
         <f>G51/G$30</f>
         <v>11222.81289297534</v>
       </c>
-      <c r="H52" s="11">
+      <c r="H52" s="10">
         <f>H51/H$30</f>
         <v>3613.6834344303147</v>
       </c>
-      <c r="I52" s="11">
+      <c r="I52" s="10">
         <f>I51/I$30</f>
         <v>11222.81289297534</v>
       </c>
-      <c r="J52" s="11">
+      <c r="J52" s="10">
         <f>J51/J$30</f>
         <v>3613.6834344303147</v>
       </c>
@@ -4338,663 +4328,663 @@
       <c r="B53" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C53" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D53" s="10" t="s">
+      <c r="C53" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
         <v>98</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" t="s">
         <v>99</v>
       </c>
-      <c r="G53" s="33">
+      <c r="G53" s="29">
         <f>G52*10^9</f>
         <v>11222812892975.34</v>
       </c>
-      <c r="H53" s="33">
+      <c r="H53" s="29">
         <f>H52*10^9</f>
         <v>3613683434430.3149</v>
       </c>
-      <c r="I53" s="33">
+      <c r="I53" s="29">
         <f>I52*10^9</f>
         <v>11222812892975.34</v>
       </c>
-      <c r="J53" s="33">
+      <c r="J53" s="29">
         <f>J52*10^9</f>
         <v>3613683434430.3149</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C54" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="D54" s="15" t="s">
+      <c r="C54" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E54" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="G54" s="43">
+      <c r="G54" s="38">
         <f>G53*G$27</f>
         <v>80655473.50496459</v>
       </c>
-      <c r="H54" s="43">
+      <c r="H54" s="38">
         <f>H53*H$27</f>
         <v>17154512.628877405</v>
       </c>
-      <c r="I54" s="43">
+      <c r="I54" s="38">
         <f>I53*I$27</f>
         <v>169376494.36042562</v>
       </c>
-      <c r="J54" s="43">
+      <c r="J54" s="38">
         <f>J53*J$27</f>
         <v>12008158.840214185</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B56" s="25" t="s">
+      <c r="B56" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C56" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D56" s="26" t="s">
+      <c r="C56" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E56" s="26" t="s">
+      <c r="E56" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F56" s="26" t="s">
+      <c r="F56" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="G56" s="29">
+      <c r="G56" s="26">
         <v>6.0221407599999999E+23</v>
       </c>
-      <c r="H56" s="29">
+      <c r="H56" s="26">
         <v>6.0221407599999999E+23</v>
       </c>
-      <c r="I56" s="29">
+      <c r="I56" s="26">
         <v>6.0221407599999999E+23</v>
       </c>
-      <c r="J56" s="29">
+      <c r="J56" s="26">
         <v>6.0221407599999999E+23</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="18" t="s">
+      <c r="B57" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C57" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D57" s="19" t="s">
+      <c r="C57" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="E57" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="F57" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G57" s="19">
+      <c r="G57" s="17">
         <v>0.54168919427718798</v>
       </c>
-      <c r="H57" s="19">
+      <c r="H57" s="17">
         <v>0.167212256132342</v>
       </c>
-      <c r="I57" s="19">
+      <c r="I57" s="17">
         <v>0.54168919427718798</v>
       </c>
-      <c r="J57" s="19">
+      <c r="J57" s="17">
         <v>0.167212256132342</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C58" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D58" s="21" t="s">
+      <c r="C58" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E58" s="21" t="s">
+      <c r="E58" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F58" s="21" t="s">
+      <c r="F58" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="G58" s="21">
+      <c r="G58" s="19">
         <v>1904788.3330000001</v>
       </c>
-      <c r="H58" s="21">
+      <c r="H58" s="19">
         <v>1904788.3330000001</v>
       </c>
-      <c r="I58" s="21">
+      <c r="I58" s="19">
         <v>1904788.3330000001</v>
       </c>
-      <c r="J58" s="21">
+      <c r="J58" s="19">
         <v>1904788.3330000001</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C59" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D59" s="21" t="s">
+      <c r="C59" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E59" s="21" t="s">
+      <c r="E59" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F59" s="21" t="s">
+      <c r="F59" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G59" s="22">
+      <c r="G59" s="20">
         <f>(G57*G$56)/(G58*G$36*10^9)</f>
         <v>263475.96007974859</v>
       </c>
-      <c r="H59" s="22">
+      <c r="H59" s="20">
         <f>(H57*H$56)/(H58*H$36*10^9)</f>
         <v>81331.527722935352</v>
       </c>
-      <c r="I59" s="22">
+      <c r="I59" s="20">
         <f>(I57*I$56)/(I58*I$36*10^9)</f>
         <v>263475.96007974859</v>
       </c>
-      <c r="J59" s="22">
+      <c r="J59" s="20">
         <f>(J57*J$56)/(J58*J$36*10^9)</f>
         <v>81331.527722935352</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C60" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D60" s="21" t="s">
+      <c r="C60" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E60" s="21" t="s">
+      <c r="E60" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F60" s="21" t="s">
+      <c r="F60" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="G60" s="21">
+      <c r="G60" s="19">
         <f>G59/G$30</f>
         <v>52695.192015949717</v>
       </c>
-      <c r="H60" s="21">
+      <c r="H60" s="19">
         <f>H59/H$30</f>
         <v>17086.455403978016</v>
       </c>
-      <c r="I60" s="21">
+      <c r="I60" s="19">
         <f>I59/I$30</f>
         <v>52695.192015949717</v>
       </c>
-      <c r="J60" s="21">
+      <c r="J60" s="19">
         <f>J59/J$30</f>
         <v>17086.455403978016</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C61" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D61" s="21" t="s">
+      <c r="C61" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E61" s="21" t="s">
+      <c r="E61" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F61" s="21" t="s">
+      <c r="F61" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G61" s="39">
+      <c r="G61" s="34">
         <f>G60*10^9</f>
         <v>52695192015949.719</v>
       </c>
-      <c r="H61" s="39">
+      <c r="H61" s="34">
         <f>H60*10^9</f>
         <v>17086455403978.016</v>
       </c>
-      <c r="I61" s="39">
+      <c r="I61" s="34">
         <f>I60*10^9</f>
         <v>52695192015949.719</v>
       </c>
-      <c r="J61" s="39">
+      <c r="J61" s="34">
         <f>J60*10^9</f>
         <v>17086455403978.016</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B62" s="23" t="s">
+      <c r="B62" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C62" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62" s="24" t="s">
+      <c r="C62" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D62" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="E62" s="24" t="s">
+      <c r="E62" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F62" s="24" t="s">
+      <c r="F62" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="G62" s="44">
+      <c r="G62" s="39">
         <f>G61*G$27</f>
         <v>378706809.42580277</v>
       </c>
-      <c r="H62" s="44">
+      <c r="H62" s="39">
         <f>H61*H$27</f>
         <v>81111093.522363067</v>
       </c>
-      <c r="I62" s="44">
+      <c r="I62" s="39">
         <f>I61*I$27</f>
         <v>795284299.79418576</v>
       </c>
-      <c r="J62" s="44">
+      <c r="J62" s="39">
         <f>J61*J$27</f>
         <v>56777765.465654157</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B63" s="25" t="s">
+      <c r="B63" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="C63" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D63" s="26" t="s">
+      <c r="C63" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D63" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="26" t="s">
+      <c r="E63" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F63" s="26" t="s">
+      <c r="F63" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G63" s="26">
+      <c r="G63" s="19">
         <v>0.65408448128256302</v>
       </c>
-      <c r="H63" s="26">
+      <c r="H63" s="19">
         <v>0.20196161687112801</v>
       </c>
-      <c r="I63" s="26">
+      <c r="I63" s="19">
         <v>0.65408448128256302</v>
       </c>
-      <c r="J63" s="26">
+      <c r="J63" s="19">
         <v>0.20196161687112801</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B64" s="26" t="s">
+      <c r="B64" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C64" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D64" s="26" t="s">
+      <c r="C64" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E64" s="26" t="s">
+      <c r="E64" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F64" s="26" t="s">
+      <c r="F64" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="G64" s="26">
+      <c r="G64" s="19">
         <v>4373730</v>
       </c>
-      <c r="H64" s="26">
+      <c r="H64" s="19">
         <v>4373730</v>
       </c>
-      <c r="I64" s="26">
+      <c r="I64" s="19">
         <v>4373730</v>
       </c>
-      <c r="J64" s="26">
+      <c r="J64" s="19">
         <v>4373730</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B65" s="26" t="s">
+      <c r="B65" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C65" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D65" s="26" t="s">
+      <c r="C65" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D65" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E65" s="26" t="s">
+      <c r="E65" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F65" s="26" t="s">
+      <c r="F65" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G65" s="22">
+      <c r="G65" s="20">
         <f>(G63*G$56)/(G64*G$36*10^9)</f>
         <v>138554.11268273849</v>
       </c>
-      <c r="H65" s="22">
+      <c r="H65" s="20">
         <f>(H63*H$56)/(H64*H$36*10^9)</f>
         <v>42781.343117452598</v>
       </c>
-      <c r="I65" s="22">
+      <c r="I65" s="20">
         <f>(I63*I$56)/(I64*I$36*10^9)</f>
         <v>138554.11268273849</v>
       </c>
-      <c r="J65" s="22">
+      <c r="J65" s="20">
         <f>(J63*J$56)/(J64*J$36*10^9)</f>
         <v>42781.343117452598</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B66" s="26" t="s">
+      <c r="B66" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C66" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D66" s="26" t="s">
+      <c r="C66" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D66" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E66" s="26" t="s">
+      <c r="E66" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F66" s="26" t="s">
+      <c r="F66" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="G66" s="26">
+      <c r="G66" s="19">
         <f>G65/G$30</f>
         <v>27710.822536547697</v>
       </c>
-      <c r="H66" s="26">
+      <c r="H66" s="19">
         <f>H65/H$30</f>
         <v>8987.6771255152526</v>
       </c>
-      <c r="I66" s="26">
+      <c r="I66" s="19">
         <f>I65/I$30</f>
         <v>27710.822536547697</v>
       </c>
-      <c r="J66" s="26">
+      <c r="J66" s="19">
         <f>J65/J$30</f>
         <v>8987.6771255152526</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B67" s="26" t="s">
+      <c r="B67" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C67" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D67" s="26" t="s">
+      <c r="C67" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D67" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E67" s="26" t="s">
+      <c r="E67" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F67" s="26" t="s">
+      <c r="F67" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G67" s="47">
+      <c r="G67" s="34">
         <f>G66*10^9</f>
         <v>27710822536547.699</v>
       </c>
-      <c r="H67" s="47">
+      <c r="H67" s="34">
         <f>H66*10^9</f>
         <v>8987677125515.252</v>
       </c>
-      <c r="I67" s="47">
+      <c r="I67" s="34">
         <f>I66*10^9</f>
         <v>27710822536547.699</v>
       </c>
-      <c r="J67" s="47">
+      <c r="J67" s="34">
         <f>J66*10^9</f>
         <v>8987677125515.252</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B68" s="26" t="s">
+      <c r="B68" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C68" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D68" s="26" t="s">
+      <c r="C68" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E68" s="26" t="s">
+      <c r="E68" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F68" s="26" t="s">
+      <c r="F68" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="G68" s="45">
+      <c r="G68" s="40">
         <f>G67*G$27</f>
         <v>199150563.60747704</v>
       </c>
-      <c r="H68" s="45">
+      <c r="H68" s="40">
         <f>H67*H$27</f>
         <v>42665392.127307303</v>
       </c>
-      <c r="I68" s="45">
+      <c r="I68" s="40">
         <f>I67*I$27</f>
         <v>418216183.57570171</v>
       </c>
-      <c r="J68" s="45">
+      <c r="J68" s="40">
         <f>J67*J$27</f>
         <v>29865774.489115112</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B69" s="18" t="s">
+      <c r="B69" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C69" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D69" s="19" t="s">
+      <c r="C69" s="17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D69" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="E69" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F69" s="19" t="s">
+      <c r="F69" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="G69" s="27">
+      <c r="G69" s="24">
         <v>5.4065556339343897E-3</v>
       </c>
-      <c r="H69" s="27">
+      <c r="H69" s="24">
         <v>1.65731861018518E-3</v>
       </c>
-      <c r="I69" s="27">
+      <c r="I69" s="24">
         <v>5.4065556339343897E-3</v>
       </c>
-      <c r="J69" s="27">
+      <c r="J69" s="24">
         <v>1.65731861018518E-3</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C70" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D70" s="21" t="s">
+      <c r="C70" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E70" s="21" t="s">
+      <c r="E70" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F70" s="21" t="s">
+      <c r="F70" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="G70" s="28">
+      <c r="G70" s="25">
         <v>89264</v>
       </c>
-      <c r="H70" s="28">
+      <c r="H70" s="25">
         <v>89264</v>
       </c>
-      <c r="I70" s="28">
+      <c r="I70" s="25">
         <v>89264</v>
       </c>
-      <c r="J70" s="28">
+      <c r="J70" s="25">
         <v>89264</v>
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C71" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D71" s="21" t="s">
+      <c r="C71" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="E71" s="21" t="s">
+      <c r="E71" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F71" s="21" t="s">
+      <c r="F71" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G71" s="22">
+      <c r="G71" s="20">
         <f>(G69*G$56)/(G70*G$36*10^9)</f>
         <v>56115.376091531296</v>
       </c>
-      <c r="H71" s="22">
+      <c r="H71" s="20">
         <f>(H69*H$56)/(H70*H$36*10^9)</f>
         <v>17201.535212236002</v>
       </c>
-      <c r="I71" s="22">
+      <c r="I71" s="20">
         <f>(I69*I$56)/(I70*I$36*10^9)</f>
         <v>56115.376091531296</v>
       </c>
-      <c r="J71" s="22">
+      <c r="J71" s="20">
         <f>(J69*J$56)/(J70*J$36*10^9)</f>
         <v>17201.535212236002</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C72" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D72" s="21" t="s">
+      <c r="C72" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D72" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E72" s="21" t="s">
+      <c r="E72" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F72" s="21" t="s">
+      <c r="F72" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="G72" s="28">
+      <c r="G72" s="25">
         <f>G71/G$30</f>
         <v>11223.07521830626</v>
       </c>
-      <c r="H72" s="28">
+      <c r="H72" s="25">
         <f>H71/H$30</f>
         <v>3613.7679017302526</v>
       </c>
-      <c r="I72" s="28">
+      <c r="I72" s="25">
         <f>I71/I$30</f>
         <v>11223.07521830626</v>
       </c>
-      <c r="J72" s="28">
+      <c r="J72" s="25">
         <f>J71/J$30</f>
         <v>3613.7679017302526</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C73" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D73" s="21" t="s">
+      <c r="C73" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D73" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E73" s="21" t="s">
+      <c r="E73" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F73" s="21" t="s">
+      <c r="F73" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G73" s="48">
+      <c r="G73" s="42">
         <f>G72*10^9</f>
         <v>11223075218306.26</v>
       </c>
-      <c r="H73" s="48">
+      <c r="H73" s="42">
         <f>H72*10^9</f>
         <v>3613767901730.2524</v>
       </c>
-      <c r="I73" s="48">
+      <c r="I73" s="42">
         <f>I72*10^9</f>
         <v>11223075218306.26</v>
       </c>
-      <c r="J73" s="48">
+      <c r="J73" s="42">
         <f>J72*10^9</f>
         <v>3613767901730.2524</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B74" s="23" t="s">
+      <c r="B74" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="C74" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="D74" s="24" t="s">
+      <c r="C74" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D74" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="E74" s="24" t="s">
+      <c r="E74" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F74" s="24" t="s">
+      <c r="F74" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="G74" s="46">
+      <c r="G74" s="41">
         <f>G73*G$27</f>
         <v>80657358.7697355</v>
       </c>
-      <c r="H74" s="46">
+      <c r="H74" s="41">
         <f>H73*H$27</f>
         <v>17154913.60350338</v>
       </c>
-      <c r="I74" s="46">
+      <c r="I74" s="41">
         <f>I73*I$27</f>
         <v>169380453.41644454</v>
       </c>
-      <c r="J74" s="46">
+      <c r="J74" s="41">
         <f>J73*J$27</f>
         <v>12008439.522452366</v>
       </c>
@@ -5013,7 +5003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A661CB-FE77-E747-9C39-6C6F06A92839}">
   <dimension ref="A1:M140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -5933,48 +5923,48 @@
     </row>
     <row r="39" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="38"/>
+      <c r="B40" s="33"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="35" t="s">
+      <c r="A41" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="35">
+      <c r="B41">
         <v>0.98650309751565746</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="35" t="s">
+      <c r="A42" t="s">
         <v>129</v>
       </c>
-      <c r="B42" s="35">
+      <c r="B42">
         <v>0.97318836140798681</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="35" t="s">
+      <c r="A43" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="35">
+      <c r="B43">
         <v>0.96983690658398514</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="35" t="s">
+      <c r="A44" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="35">
+      <c r="B44">
         <v>0.25889978076474535</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="36">
+      <c r="B45" s="31">
         <v>10</v>
       </c>
     </row>
@@ -5984,156 +5974,154 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="37"/>
-      <c r="B48" s="37" t="s">
+      <c r="A48" s="32"/>
+      <c r="B48" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="37" t="s">
+      <c r="C48" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E48" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="F48" s="37" t="s">
+      <c r="F48" s="32" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="35" t="s">
+      <c r="A49" t="s">
         <v>134</v>
       </c>
-      <c r="B49" s="35">
-        <v>1</v>
-      </c>
-      <c r="C49" s="35">
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
         <v>19.463767228159732</v>
       </c>
-      <c r="D49" s="35">
+      <c r="D49">
         <v>19.463767228159732</v>
       </c>
-      <c r="E49" s="35">
+      <c r="E49">
         <v>290.37788438574057</v>
       </c>
-      <c r="F49" s="35">
+      <c r="F49">
         <v>1.4284435606597672E-7</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="35" t="s">
+      <c r="A50" t="s">
         <v>135</v>
       </c>
-      <c r="B50" s="35">
+      <c r="B50">
         <v>8</v>
       </c>
-      <c r="C50" s="35">
+      <c r="C50">
         <v>0.53623277184026563</v>
       </c>
-      <c r="D50" s="35">
+      <c r="D50">
         <v>6.7029096480033204E-2</v>
       </c>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
     </row>
     <row r="51" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="B51" s="36">
+      <c r="B51" s="31">
         <v>9</v>
       </c>
-      <c r="C51" s="36">
+      <c r="C51" s="31">
         <v>19.999999999999996</v>
       </c>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
     </row>
     <row r="52" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="37"/>
-      <c r="B53" s="37" t="s">
+      <c r="A53" s="32"/>
+      <c r="B53" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="C53" s="37" t="s">
+      <c r="C53" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="D53" s="37" t="s">
+      <c r="D53" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="E53" s="37" t="s">
+      <c r="E53" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="F53" s="37" t="s">
+      <c r="F53" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="G53" s="37" t="s">
+      <c r="G53" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="H53" s="37" t="s">
+      <c r="H53" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="I53" s="37" t="s">
+      <c r="I53" s="32" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="35" t="s">
+      <c r="A54" t="s">
         <v>137</v>
       </c>
-      <c r="B54" s="35">
+      <c r="B54">
         <v>-6.7242381884894638</v>
       </c>
-      <c r="C54" s="35">
+      <c r="C54">
         <v>0.2361976278251447</v>
       </c>
-      <c r="D54" s="35">
+      <c r="D54">
         <v>-28.46869484001493</v>
       </c>
-      <c r="E54" s="35">
+      <c r="E54">
         <v>2.5056435242303998E-9</v>
       </c>
-      <c r="F54" s="35">
+      <c r="F54">
         <v>-7.2689108949796619</v>
       </c>
-      <c r="G54" s="35">
+      <c r="G54">
         <v>-6.1795654819992656</v>
       </c>
-      <c r="H54" s="35">
+      <c r="H54">
         <v>-7.2689108949796619</v>
       </c>
-      <c r="I54" s="35">
+      <c r="I54">
         <v>-6.1795654819992656</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="36" t="s">
+      <c r="A55" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="B55" s="36">
+      <c r="B55" s="31">
         <v>1.2448765237913186</v>
       </c>
-      <c r="C55" s="36">
+      <c r="C55" s="31">
         <v>7.3054085503350158E-2</v>
       </c>
-      <c r="D55" s="36">
+      <c r="D55" s="31">
         <v>17.040477821520746</v>
       </c>
-      <c r="E55" s="36">
+      <c r="E55" s="31">
         <v>1.4284435606597722E-7</v>
       </c>
-      <c r="F55" s="36">
+      <c r="F55" s="31">
         <v>1.0764135005270343</v>
       </c>
-      <c r="G55" s="36">
+      <c r="G55" s="31">
         <v>1.4133395470556029</v>
       </c>
-      <c r="H55" s="36">
+      <c r="H55" s="31">
         <v>1.0764135005270343</v>
       </c>
-      <c r="I55" s="36">
+      <c r="I55" s="31">
         <v>1.4133395470556029</v>
       </c>
     </row>
@@ -6149,48 +6137,48 @@
     </row>
     <row r="60" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="38" t="s">
+      <c r="A61" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B61" s="38"/>
+      <c r="B61" s="33"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="35" t="s">
+      <c r="A62" t="s">
         <v>128</v>
       </c>
-      <c r="B62" s="35">
+      <c r="B62">
         <v>0.98632417973563269</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="35" t="s">
+      <c r="A63" t="s">
         <v>129</v>
       </c>
-      <c r="B63" s="35">
+      <c r="B63">
         <v>0.9728353875311686</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="35" t="s">
+      <c r="A64" t="s">
         <v>130</v>
       </c>
-      <c r="B64" s="35">
+      <c r="B64">
         <v>0.9694398109725646</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" s="35" t="s">
+      <c r="A65" t="s">
         <v>131</v>
       </c>
-      <c r="B65" s="35">
+      <c r="B65">
         <v>0.26059840976506049</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="36" t="s">
+      <c r="A66" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="B66" s="36">
+      <c r="B66" s="31">
         <v>10</v>
       </c>
     </row>
@@ -6200,156 +6188,154 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="37"/>
-      <c r="B69" s="37" t="s">
+      <c r="A69" s="32"/>
+      <c r="B69" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="C69" s="37" t="s">
+      <c r="C69" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="D69" s="37" t="s">
+      <c r="D69" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="E69" s="37" t="s">
+      <c r="E69" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="F69" s="37" t="s">
+      <c r="F69" s="32" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" s="35" t="s">
+      <c r="A70" t="s">
         <v>134</v>
       </c>
-      <c r="B70" s="35">
-        <v>1</v>
-      </c>
-      <c r="C70" s="35">
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
         <v>19.456707750623369</v>
       </c>
-      <c r="D70" s="35">
+      <c r="D70">
         <v>19.456707750623369</v>
       </c>
-      <c r="E70" s="35">
+      <c r="E70">
         <v>286.50079618029497</v>
       </c>
-      <c r="F70" s="35">
+      <c r="F70">
         <v>1.5053811468097101E-7</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="35" t="s">
+      <c r="A71" t="s">
         <v>135</v>
       </c>
-      <c r="B71" s="35">
+      <c r="B71">
         <v>8</v>
       </c>
-      <c r="C71" s="35">
+      <c r="C71">
         <v>0.5432922493766269</v>
       </c>
-      <c r="D71" s="35">
+      <c r="D71">
         <v>6.7911531172078363E-2</v>
       </c>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
     </row>
     <row r="72" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="36" t="s">
+      <c r="A72" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="B72" s="36">
+      <c r="B72" s="31">
         <v>9</v>
       </c>
-      <c r="C72" s="36">
+      <c r="C72" s="31">
         <v>19.999999999999996</v>
       </c>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
+      <c r="D72" s="31"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="31"/>
     </row>
     <row r="73" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" s="37"/>
-      <c r="B74" s="37" t="s">
+      <c r="A74" s="32"/>
+      <c r="B74" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="C74" s="37" t="s">
+      <c r="C74" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="D74" s="37" t="s">
+      <c r="D74" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="E74" s="37" t="s">
+      <c r="E74" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="F74" s="37" t="s">
+      <c r="F74" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="G74" s="37" t="s">
+      <c r="G74" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="H74" s="37" t="s">
+      <c r="H74" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="I74" s="37" t="s">
+      <c r="I74" s="32" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" s="35" t="s">
+      <c r="A75" t="s">
         <v>137</v>
       </c>
-      <c r="B75" s="35">
+      <c r="B75">
         <v>-7.1553189737083844</v>
       </c>
-      <c r="C75" s="35">
+      <c r="C75">
         <v>0.25639567558447424</v>
       </c>
-      <c r="D75" s="35">
+      <c r="D75">
         <v>-27.907330953992375</v>
       </c>
-      <c r="E75" s="35">
+      <c r="E75">
         <v>2.9342178761498629E-9</v>
       </c>
-      <c r="F75" s="35">
+      <c r="F75">
         <v>-7.7465684618546478</v>
       </c>
-      <c r="G75" s="35">
+      <c r="G75">
         <v>-6.5640694855621211</v>
       </c>
-      <c r="H75" s="35">
+      <c r="H75">
         <v>-7.7465684618546478</v>
       </c>
-      <c r="I75" s="35">
+      <c r="I75">
         <v>-6.5640694855621211</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="36" t="s">
+      <c r="A76" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="B76" s="36">
+      <c r="B76" s="31">
         <v>1.24675913604407</v>
       </c>
-      <c r="C76" s="36">
+      <c r="C76" s="31">
         <v>7.3657952553024028E-2</v>
       </c>
-      <c r="D76" s="36">
+      <c r="D76" s="31">
         <v>16.926334398808702</v>
       </c>
-      <c r="E76" s="36">
+      <c r="E76" s="31">
         <v>1.505381146809713E-7</v>
       </c>
-      <c r="F76" s="36">
+      <c r="F76" s="31">
         <v>1.0769035928661241</v>
       </c>
-      <c r="G76" s="36">
+      <c r="G76" s="31">
         <v>1.4166146792220158</v>
       </c>
-      <c r="H76" s="36">
+      <c r="H76" s="31">
         <v>1.0769035928661241</v>
       </c>
-      <c r="I76" s="36">
+      <c r="I76" s="31">
         <v>1.4166146792220158</v>
       </c>
     </row>
@@ -7125,48 +7111,48 @@
     </row>
     <row r="103" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A104" s="38" t="s">
+      <c r="A104" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B104" s="38"/>
+      <c r="B104" s="33"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A105" s="35" t="s">
+      <c r="A105" t="s">
         <v>128</v>
       </c>
-      <c r="B105" s="35">
+      <c r="B105">
         <v>0.98277768956987499</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A106" s="35" t="s">
+      <c r="A106" t="s">
         <v>129</v>
       </c>
-      <c r="B106" s="35">
+      <c r="B106">
         <v>0.96585198711630149</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A107" s="35" t="s">
+      <c r="A107" t="s">
         <v>130</v>
       </c>
-      <c r="B107" s="35">
+      <c r="B107">
         <v>0.96097369956148737</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A108" s="35" t="s">
+      <c r="A108" t="s">
         <v>131</v>
       </c>
-      <c r="B108" s="35">
+      <c r="B108">
         <v>0.27547136525396865</v>
       </c>
     </row>
     <row r="109" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="36" t="s">
+      <c r="A109" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="B109" s="36">
+      <c r="B109" s="31">
         <v>9</v>
       </c>
     </row>
@@ -7176,156 +7162,154 @@
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A112" s="37"/>
-      <c r="B112" s="37" t="s">
+      <c r="A112" s="32"/>
+      <c r="B112" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="C112" s="37" t="s">
+      <c r="C112" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="D112" s="37" t="s">
+      <c r="D112" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="E112" s="37" t="s">
+      <c r="E112" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="F112" s="37" t="s">
+      <c r="F112" s="32" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A113" s="35" t="s">
+      <c r="A113" t="s">
         <v>134</v>
       </c>
-      <c r="B113" s="35">
-        <v>1</v>
-      </c>
-      <c r="C113" s="35">
+      <c r="B113">
+        <v>1</v>
+      </c>
+      <c r="C113">
         <v>15.024364244031355</v>
       </c>
-      <c r="D113" s="35">
+      <c r="D113">
         <v>15.024364244031355</v>
       </c>
-      <c r="E113" s="35">
+      <c r="E113">
         <v>197.98996600009067</v>
       </c>
-      <c r="F113" s="35">
+      <c r="F113">
         <v>2.170514370853631E-6</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A114" s="35" t="s">
+      <c r="A114" t="s">
         <v>135</v>
       </c>
-      <c r="B114" s="35">
+      <c r="B114">
         <v>7</v>
       </c>
-      <c r="C114" s="35">
+      <c r="C114">
         <v>0.53119131152419774</v>
       </c>
-      <c r="D114" s="35">
+      <c r="D114">
         <v>7.5884473074885397E-2</v>
       </c>
-      <c r="E114" s="35"/>
-      <c r="F114" s="35"/>
     </row>
     <row r="115" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="36" t="s">
+      <c r="A115" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="B115" s="36">
+      <c r="B115" s="31">
         <v>8</v>
       </c>
-      <c r="C115" s="36">
+      <c r="C115" s="31">
         <v>15.555555555555554</v>
       </c>
-      <c r="D115" s="36"/>
-      <c r="E115" s="36"/>
-      <c r="F115" s="36"/>
+      <c r="D115" s="31"/>
+      <c r="E115" s="31"/>
+      <c r="F115" s="31"/>
     </row>
     <row r="116" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="117" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A117" s="37"/>
-      <c r="B117" s="37" t="s">
+      <c r="A117" s="32"/>
+      <c r="B117" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="C117" s="37" t="s">
+      <c r="C117" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="D117" s="37" t="s">
+      <c r="D117" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="E117" s="37" t="s">
+      <c r="E117" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="F117" s="37" t="s">
+      <c r="F117" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="G117" s="37" t="s">
+      <c r="G117" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="H117" s="37" t="s">
+      <c r="H117" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="I117" s="37" t="s">
+      <c r="I117" s="32" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A118" s="35" t="s">
+      <c r="A118" t="s">
         <v>137</v>
       </c>
-      <c r="B118" s="35">
+      <c r="B118">
         <v>-6.7671601206840846</v>
       </c>
-      <c r="C118" s="35">
+      <c r="C118">
         <v>0.30147987595768366</v>
       </c>
-      <c r="D118" s="35">
+      <c r="D118">
         <v>-22.44647374617448</v>
       </c>
-      <c r="E118" s="35">
+      <c r="E118">
         <v>8.8123820173190667E-8</v>
       </c>
-      <c r="F118" s="35">
+      <c r="F118">
         <v>-7.4800467467408076</v>
       </c>
-      <c r="G118" s="35">
+      <c r="G118">
         <v>-6.0542734946273615</v>
       </c>
-      <c r="H118" s="35">
+      <c r="H118">
         <v>-7.4800467467408076</v>
       </c>
-      <c r="I118" s="35">
+      <c r="I118">
         <v>-6.0542734946273615</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="36" t="s">
+      <c r="A119" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="B119" s="36">
+      <c r="B119" s="31">
         <v>1.2561949109446751</v>
       </c>
-      <c r="C119" s="36">
+      <c r="C119" s="31">
         <v>8.9276147107148096E-2</v>
       </c>
-      <c r="D119" s="36">
+      <c r="D119" s="31">
         <v>14.070890732291637</v>
       </c>
-      <c r="E119" s="36">
+      <c r="E119" s="31">
         <v>2.170514370853631E-6</v>
       </c>
-      <c r="F119" s="36">
+      <c r="F119" s="31">
         <v>1.0450903684063477</v>
       </c>
-      <c r="G119" s="36">
+      <c r="G119" s="31">
         <v>1.4672994534830024</v>
       </c>
-      <c r="H119" s="36">
+      <c r="H119" s="31">
         <v>1.0450903684063477</v>
       </c>
-      <c r="I119" s="36">
+      <c r="I119" s="31">
         <v>1.4672994534830024</v>
       </c>
     </row>
@@ -7341,48 +7325,48 @@
     </row>
     <row r="124" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="125" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A125" s="38" t="s">
+      <c r="A125" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="B125" s="38"/>
+      <c r="B125" s="33"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A126" s="35" t="s">
+      <c r="A126" t="s">
         <v>128</v>
       </c>
-      <c r="B126" s="35">
+      <c r="B126">
         <v>0.98251270102667276</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A127" s="35" t="s">
+      <c r="A127" t="s">
         <v>129</v>
       </c>
-      <c r="B127" s="35">
+      <c r="B127">
         <v>0.96533120767872804</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A128" s="35" t="s">
+      <c r="A128" t="s">
         <v>130</v>
       </c>
-      <c r="B128" s="35">
+      <c r="B128">
         <v>0.96037852306140348</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A129" s="35" t="s">
+      <c r="A129" t="s">
         <v>131</v>
       </c>
-      <c r="B129" s="35">
+      <c r="B129">
         <v>0.2775639758937346</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="36" t="s">
+      <c r="A130" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="B130" s="36">
+      <c r="B130" s="31">
         <v>9</v>
       </c>
     </row>
@@ -7392,156 +7376,154 @@
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A133" s="37"/>
-      <c r="B133" s="37" t="s">
+      <c r="A133" s="32"/>
+      <c r="B133" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="C133" s="37" t="s">
+      <c r="C133" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="D133" s="37" t="s">
+      <c r="D133" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="E133" s="37" t="s">
+      <c r="E133" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="F133" s="37" t="s">
+      <c r="F133" s="32" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A134" s="35" t="s">
+      <c r="A134" t="s">
         <v>134</v>
       </c>
-      <c r="B134" s="35">
-        <v>1</v>
-      </c>
-      <c r="C134" s="35">
+      <c r="B134">
+        <v>1</v>
+      </c>
+      <c r="C134">
         <v>15.016263230557989</v>
       </c>
-      <c r="D134" s="35">
+      <c r="D134">
         <v>15.016263230557989</v>
       </c>
-      <c r="E134" s="35">
+      <c r="E134">
         <v>194.91069637303065</v>
       </c>
-      <c r="F134" s="35">
+      <c r="F134">
         <v>2.2890733334159977E-6</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A135" s="35" t="s">
+      <c r="A135" t="s">
         <v>135</v>
       </c>
-      <c r="B135" s="35">
+      <c r="B135">
         <v>7</v>
       </c>
-      <c r="C135" s="35">
+      <c r="C135">
         <v>0.53929232499756385</v>
       </c>
-      <c r="D135" s="35">
+      <c r="D135">
         <v>7.7041760713937688E-2</v>
       </c>
-      <c r="E135" s="35"/>
-      <c r="F135" s="35"/>
     </row>
     <row r="136" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="36" t="s">
+      <c r="A136" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="B136" s="36">
+      <c r="B136" s="31">
         <v>8</v>
       </c>
-      <c r="C136" s="36">
+      <c r="C136" s="31">
         <v>15.555555555555554</v>
       </c>
-      <c r="D136" s="36"/>
-      <c r="E136" s="36"/>
-      <c r="F136" s="36"/>
+      <c r="D136" s="31"/>
+      <c r="E136" s="31"/>
+      <c r="F136" s="31"/>
     </row>
     <row r="137" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="138" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A138" s="37"/>
-      <c r="B138" s="37" t="s">
+      <c r="A138" s="32"/>
+      <c r="B138" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="C138" s="37" t="s">
+      <c r="C138" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="D138" s="37" t="s">
+      <c r="D138" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="E138" s="37" t="s">
+      <c r="E138" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="F138" s="37" t="s">
+      <c r="F138" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="G138" s="37" t="s">
+      <c r="G138" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="H138" s="37" t="s">
+      <c r="H138" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="I138" s="37" t="s">
+      <c r="I138" s="32" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A139" s="35" t="s">
+      <c r="A139" t="s">
         <v>137</v>
       </c>
-      <c r="B139" s="35">
+      <c r="B139">
         <v>-7.1961286730013798</v>
       </c>
-      <c r="C139" s="35">
+      <c r="C139">
         <v>0.32657986324660049</v>
       </c>
-      <c r="D139" s="35">
+      <c r="D139">
         <v>-22.034820522806033</v>
       </c>
-      <c r="E139" s="35">
+      <c r="E139">
         <v>1.0015331226030484E-7</v>
       </c>
-      <c r="F139" s="35">
+      <c r="F139">
         <v>-7.9683673377161464</v>
       </c>
-      <c r="G139" s="35">
+      <c r="G139">
         <v>-6.4238900082866133</v>
       </c>
-      <c r="H139" s="35">
+      <c r="H139">
         <v>-7.9683673377161464</v>
       </c>
-      <c r="I139" s="35">
+      <c r="I139">
         <v>-6.4238900082866133</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="36" t="s">
+      <c r="A140" s="31" t="s">
         <v>166</v>
       </c>
-      <c r="B140" s="36">
+      <c r="B140" s="31">
         <v>1.2568191864801974</v>
       </c>
-      <c r="C140" s="36">
+      <c r="C140" s="31">
         <v>9.0023307568673744E-2</v>
       </c>
-      <c r="D140" s="36">
+      <c r="D140" s="31">
         <v>13.961042094809063</v>
       </c>
-      <c r="E140" s="36">
+      <c r="E140" s="31">
         <v>2.2890733334160024E-6</v>
       </c>
-      <c r="F140" s="36">
+      <c r="F140" s="31">
         <v>1.0439478901947152</v>
       </c>
-      <c r="G140" s="36">
+      <c r="G140" s="31">
         <v>1.4696904827656796</v>
       </c>
-      <c r="H140" s="36">
+      <c r="H140" s="31">
         <v>1.0439478901947152</v>
       </c>
-      <c r="I140" s="36">
+      <c r="I140" s="31">
         <v>1.4696904827656796</v>
       </c>
     </row>
@@ -7571,7 +7553,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="43" t="s">
         <v>207</v>
       </c>
     </row>

</xml_diff>